<commit_message>
StatusComponent 쪼개기, BoxComponent 추가, UI 수정
</commit_message>
<xml_diff>
--- a/Design/Excels/ItemTable.xlsx
+++ b/Design/Excels/ItemTable.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JH\UnityProjects\BeautifulDeathMatch\Beautiful-DeathMatch\Design\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE32F983-0DD2-44A7-B9E9-6B73D54D2FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A502967-6C2B-4EC9-82A8-3B2AFD13590E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3972" yWindow="2148" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="2016" windowWidth="23040" windowHeight="12204" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
     <sheet name="ItemType" sheetId="2" r:id="rId2"/>
     <sheet name="ItemPosition" sheetId="3" r:id="rId3"/>
     <sheet name="ItemStartingPlayer" sheetId="4" r:id="rId4"/>
-    <sheet name="StringKey" sheetId="5" r:id="rId5"/>
+    <sheet name="BoxData" sheetId="6" r:id="rId5"/>
+    <sheet name="BoxStarting" sheetId="7" r:id="rId6"/>
+    <sheet name="StringKey" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -197,6 +199,18 @@
   </si>
   <si>
     <t>en6</t>
+  </si>
+  <si>
+    <t>boxId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>areaIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -681,10 +695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7041EE0-3748-4342-B006-84740D2969E0}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -821,6 +835,102 @@
         <v>25</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>201</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>202</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>203</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>204</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>206</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>301</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>302</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>303</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>304</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>305</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>306</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -831,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC0A8C0-25A6-4D9E-869F-200329E1AA6D}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1187,6 +1297,189 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365E39BD-9FDD-4437-A01B-D4B0A9DFF3BA}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="21.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>201</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>202</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>203</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>204</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>205</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>206</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>301</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>302</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>303</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>304</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>305</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>306</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693776E6-5BD6-4F87-B95B-F4A4876A1AC8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E390BA2F-98DF-4E9B-B8EA-7EEE2DEF3255}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>